<commit_message>
Last Commit for Demo
</commit_message>
<xml_diff>
--- a/src/main/java/com/absli/testdata/client/organization/Test Data For TC_CO_001.xlsx
+++ b/src/main/java/com/absli/testdata/client/organization/Test Data For TC_CO_001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gokulnath\Desktop\Test Data\Client Organization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gokulnath\git\com.absli.auto\src\main\java\com\absli\testdata\client\organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -458,7 +458,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>